<commit_message>
Revisione generazione istanze ed euristica
</commit_message>
<xml_diff>
--- a/All_facilities.xlsx
+++ b/All_facilities.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,21 +462,21 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SIECO S.R.L.</t>
+          <t>INNOCENTI SRL</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>42.4539311</v>
+        <v>41.955471</v>
       </c>
       <c r="E2" t="n">
-        <v>12.0871977</v>
+        <v>12.7640919</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -486,21 +486,21 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>965</v>
+        <v>10</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MEDIASERVICE RECYCLING SRL</t>
+          <t>FITALS S.R.L.</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>41.9319972</v>
+        <v>41.9404295</v>
       </c>
       <c r="E3" t="n">
-        <v>12.6140927</v>
+        <v>12.632209</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -558,21 +558,21 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>FITALS S.R.L.</t>
+          <t>GE.SER. SRL</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>41.9404295</v>
+        <v>41.9507218</v>
       </c>
       <c r="E6" t="n">
-        <v>12.632209</v>
+        <v>12.7554548</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -582,21 +582,21 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2134</v>
+        <v>81</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ECO LOGICA 2000 SRL</t>
+          <t>RECYCLING PFU SRL</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>41.7931483</v>
+        <v>41.2759554</v>
       </c>
       <c r="E7" t="n">
-        <v>12.5359218</v>
+        <v>13.7880158</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -606,21 +606,21 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RECYCLING PFU SRL</t>
+          <t>RICREA SRL</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>41.2759554</v>
+        <v>41.7082726</v>
       </c>
       <c r="E8" t="n">
-        <v>13.7880158</v>
+        <v>12.5870176</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -630,21 +630,21 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>68</v>
+        <v>205</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GE.SER. SRL</t>
+          <t>SIECO S.R.L.</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>41.9507218</v>
+        <v>42.4539311</v>
       </c>
       <c r="E9" t="n">
-        <v>12.7554548</v>
+        <v>12.0871977</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -654,21 +654,21 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>211</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>INNOCENTI SRL</t>
+          <t>RIME 1</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>41.955471</v>
+        <v>41.8345359</v>
       </c>
       <c r="E10" t="n">
-        <v>12.7640919</v>
+        <v>12.4310169</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -678,23 +678,407 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>211</v>
+        <v>270</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>RIME 1</t>
+          <t>ECOLOGIC SYSTEM COMPANY SRL</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>41.8345359</v>
+        <v>41.6942634</v>
       </c>
       <c r="E11" t="n">
-        <v>12.4310169</v>
+        <v>12.534113</v>
       </c>
       <c r="F11" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>349</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CE.STRA SRL</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>41.8479537</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12.6346416</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>441</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>FEROCART SRL</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>41.89457</v>
+      </c>
+      <c r="E13" t="n">
+        <v>12.37798</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>484</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SIDERURGICA TIBURTINA S.R.L.</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>41.9602459</v>
+      </c>
+      <c r="E14" t="n">
+        <v>12.7015494</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>524</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SO.GE.RI.T SRL</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>41.4132753</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13.1695125</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>663</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>N.I.ECO S.P.A.</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>41.9271213</v>
+      </c>
+      <c r="E16" t="n">
+        <v>12.6238636</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>772</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>RICICLA CENTRO ITALIA SRL</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>41.8842861</v>
+      </c>
+      <c r="E17" t="n">
+        <v>12.704119</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>965</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>MEDIASERVICE RECYCLING SRL</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>41.9319972</v>
+      </c>
+      <c r="E18" t="n">
+        <v>12.6140927</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1368</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ECO LOGICA 2000 SRL</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>41.7824934</v>
+      </c>
+      <c r="E19" t="n">
+        <v>12.604908</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2134</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ECO LOGICA 2000 SRL</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>41.7931483</v>
+      </c>
+      <c r="E20" t="n">
+        <v>12.5359218</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3258</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>IBIOS SRL</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>42.0461171</v>
+      </c>
+      <c r="E21" t="n">
+        <v>12.5552946</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3403</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>EASY TONER SNC</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>41.9743277</v>
+      </c>
+      <c r="E22" t="n">
+        <v>12.5075322</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B23" t="n">
+        <v>4134</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SE.IN SRL</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>41.64394920000001</v>
+      </c>
+      <c r="E23" t="n">
+        <v>13.2197606</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B24" t="n">
+        <v>4763</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CARLUCCIO ROTTAMI DI ROCCA &amp; C.SNC</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>41.955343</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12.765942</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B25" t="n">
+        <v>4881</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>FITALS SRL</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>41.9404295</v>
+      </c>
+      <c r="E25" t="n">
+        <v>12.632209</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B26" t="n">
+        <v>5463</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ECOSYSTEM SPA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>41.7064274</v>
+      </c>
+      <c r="E26" t="n">
+        <v>12.5457223</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B27" t="n">
+        <v>6826</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>TECNOGARDEN SERVICE SRL</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>41.8916652</v>
+      </c>
+      <c r="E27" t="n">
+        <v>12.6232211</v>
+      </c>
+      <c r="F27" t="inlineStr">
         <is>
           <t>facility</t>
         </is>

</xml_diff>